<commit_message>
Updated to include option to allow transcoding smallest first
</commit_message>
<xml_diff>
--- a/log_compare_transcode_options_results.xlsx
+++ b/log_compare_transcode_options_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dan Documents\eclipse_workspace\run_ffmpeg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB619205-52C3-483F-B644-24EA4A2D1FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06D97FB-0DEF-4C00-B8F8-7622D79B0D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{CD55235F-E2F2-4909-81A8-9F107627486B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{CD55235F-E2F2-4909-81A8-9F107627486B}"/>
   </bookViews>
   <sheets>
     <sheet name="Observations" sheetId="11" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1464,7 +1464,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1477,14 +1477,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -19874,6 +19873,1385 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FEB77646-3DBA-4492-8253-31CBB347E50E}" name="PivotTable14" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="F39:H46" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="5"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Input File Size" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Output File Size" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="6">
+    <format dxfId="5">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="4">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="3">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="2">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="0">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A0A28DC8-6D37-401F-9D67-74AD0D675A0F}" name="PivotTable10" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="F29:I37" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="10">
+        <item sd="0" x="4"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="0"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="8"/>
+        <item t="default" sd="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item sd="0" x="5"/>
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="252">
+        <item x="208"/>
+        <item x="211"/>
+        <item x="213"/>
+        <item x="215"/>
+        <item x="217"/>
+        <item x="209"/>
+        <item x="196"/>
+        <item x="200"/>
+        <item x="202"/>
+        <item x="204"/>
+        <item x="206"/>
+        <item x="198"/>
+        <item x="219"/>
+        <item x="223"/>
+        <item x="225"/>
+        <item x="227"/>
+        <item x="229"/>
+        <item x="221"/>
+        <item x="231"/>
+        <item x="236"/>
+        <item x="238"/>
+        <item x="240"/>
+        <item x="242"/>
+        <item x="233"/>
+        <item x="244"/>
+        <item x="248"/>
+        <item x="250"/>
+        <item x="246"/>
+        <item x="172"/>
+        <item x="176"/>
+        <item x="178"/>
+        <item x="180"/>
+        <item x="182"/>
+        <item x="174"/>
+        <item x="160"/>
+        <item x="164"/>
+        <item x="166"/>
+        <item x="168"/>
+        <item x="170"/>
+        <item x="162"/>
+        <item x="184"/>
+        <item x="188"/>
+        <item x="190"/>
+        <item x="192"/>
+        <item x="194"/>
+        <item x="186"/>
+        <item x="234"/>
+        <item x="212"/>
+        <item x="214"/>
+        <item x="216"/>
+        <item x="218"/>
+        <item x="210"/>
+        <item x="197"/>
+        <item x="201"/>
+        <item x="203"/>
+        <item x="205"/>
+        <item x="207"/>
+        <item x="199"/>
+        <item x="220"/>
+        <item x="224"/>
+        <item x="226"/>
+        <item x="228"/>
+        <item x="230"/>
+        <item x="222"/>
+        <item x="232"/>
+        <item x="237"/>
+        <item x="239"/>
+        <item x="241"/>
+        <item x="243"/>
+        <item x="235"/>
+        <item x="245"/>
+        <item x="249"/>
+        <item x="247"/>
+        <item x="173"/>
+        <item x="177"/>
+        <item x="179"/>
+        <item x="181"/>
+        <item x="183"/>
+        <item x="175"/>
+        <item x="161"/>
+        <item x="165"/>
+        <item x="167"/>
+        <item x="169"/>
+        <item x="171"/>
+        <item x="163"/>
+        <item x="185"/>
+        <item x="189"/>
+        <item x="191"/>
+        <item x="193"/>
+        <item x="195"/>
+        <item x="187"/>
+        <item x="23"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="24"/>
+        <item x="17"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="18"/>
+        <item x="29"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="30"/>
+        <item x="35"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="36"/>
+        <item x="41"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="42"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="12"/>
+        <item x="47"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="48"/>
+        <item x="100"/>
+        <item x="104"/>
+        <item x="106"/>
+        <item x="108"/>
+        <item x="110"/>
+        <item x="102"/>
+        <item x="88"/>
+        <item x="92"/>
+        <item x="94"/>
+        <item x="96"/>
+        <item x="98"/>
+        <item x="90"/>
+        <item x="112"/>
+        <item x="116"/>
+        <item x="118"/>
+        <item x="120"/>
+        <item x="122"/>
+        <item x="114"/>
+        <item x="124"/>
+        <item x="128"/>
+        <item x="130"/>
+        <item x="132"/>
+        <item x="134"/>
+        <item x="126"/>
+        <item x="136"/>
+        <item x="140"/>
+        <item x="142"/>
+        <item x="144"/>
+        <item x="146"/>
+        <item x="138"/>
+        <item x="64"/>
+        <item x="68"/>
+        <item x="70"/>
+        <item x="72"/>
+        <item x="74"/>
+        <item x="66"/>
+        <item x="56"/>
+        <item x="58"/>
+        <item x="60"/>
+        <item x="62"/>
+        <item x="54"/>
+        <item x="76"/>
+        <item x="80"/>
+        <item x="82"/>
+        <item x="84"/>
+        <item x="86"/>
+        <item x="78"/>
+        <item x="148"/>
+        <item x="152"/>
+        <item x="154"/>
+        <item x="156"/>
+        <item x="158"/>
+        <item x="150"/>
+        <item x="101"/>
+        <item x="105"/>
+        <item x="107"/>
+        <item x="109"/>
+        <item x="111"/>
+        <item x="103"/>
+        <item x="89"/>
+        <item x="93"/>
+        <item x="95"/>
+        <item x="97"/>
+        <item x="99"/>
+        <item x="91"/>
+        <item x="113"/>
+        <item x="117"/>
+        <item x="119"/>
+        <item x="121"/>
+        <item x="123"/>
+        <item x="115"/>
+        <item x="125"/>
+        <item x="129"/>
+        <item x="131"/>
+        <item x="133"/>
+        <item x="135"/>
+        <item x="127"/>
+        <item x="137"/>
+        <item x="141"/>
+        <item x="143"/>
+        <item x="145"/>
+        <item x="147"/>
+        <item x="139"/>
+        <item x="65"/>
+        <item x="69"/>
+        <item x="71"/>
+        <item x="73"/>
+        <item x="75"/>
+        <item x="67"/>
+        <item x="53"/>
+        <item x="57"/>
+        <item x="59"/>
+        <item x="61"/>
+        <item x="63"/>
+        <item x="55"/>
+        <item x="77"/>
+        <item x="81"/>
+        <item x="83"/>
+        <item x="85"/>
+        <item x="87"/>
+        <item x="79"/>
+        <item x="149"/>
+        <item x="153"/>
+        <item x="155"/>
+        <item x="157"/>
+        <item x="159"/>
+        <item x="151"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="3"/>
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Time Per GB" fld="8" subtotal="average" baseField="3" baseItem="5" numFmtId="164"/>
+  </dataFields>
+  <formats count="9">
+    <format dxfId="14">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="13">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="12">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="11">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="10">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="9">
+      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0"/>
+    </format>
+    <format dxfId="8">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="7">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E287444A-7E03-49CE-AE53-6E5021066FC9}" name="PivotTable6" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+  <location ref="A2:D13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="10">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item t="default" sd="0"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="252">
+        <item x="208"/>
+        <item x="211"/>
+        <item x="213"/>
+        <item x="215"/>
+        <item x="217"/>
+        <item x="209"/>
+        <item x="196"/>
+        <item x="200"/>
+        <item x="202"/>
+        <item x="204"/>
+        <item x="206"/>
+        <item x="198"/>
+        <item x="219"/>
+        <item x="223"/>
+        <item x="225"/>
+        <item x="227"/>
+        <item x="229"/>
+        <item x="221"/>
+        <item x="231"/>
+        <item x="236"/>
+        <item x="238"/>
+        <item x="240"/>
+        <item x="242"/>
+        <item x="233"/>
+        <item x="244"/>
+        <item x="248"/>
+        <item x="250"/>
+        <item x="246"/>
+        <item x="172"/>
+        <item x="176"/>
+        <item x="178"/>
+        <item x="180"/>
+        <item x="182"/>
+        <item x="174"/>
+        <item x="160"/>
+        <item x="164"/>
+        <item x="166"/>
+        <item x="168"/>
+        <item x="170"/>
+        <item x="162"/>
+        <item x="184"/>
+        <item x="188"/>
+        <item x="190"/>
+        <item x="192"/>
+        <item x="194"/>
+        <item x="186"/>
+        <item x="234"/>
+        <item x="212"/>
+        <item x="214"/>
+        <item x="216"/>
+        <item x="218"/>
+        <item x="210"/>
+        <item x="197"/>
+        <item x="201"/>
+        <item x="203"/>
+        <item x="205"/>
+        <item x="207"/>
+        <item x="199"/>
+        <item x="220"/>
+        <item x="224"/>
+        <item x="226"/>
+        <item x="228"/>
+        <item x="230"/>
+        <item x="222"/>
+        <item x="232"/>
+        <item x="237"/>
+        <item x="239"/>
+        <item x="241"/>
+        <item x="243"/>
+        <item x="235"/>
+        <item x="245"/>
+        <item x="249"/>
+        <item x="247"/>
+        <item x="173"/>
+        <item x="177"/>
+        <item x="179"/>
+        <item x="181"/>
+        <item x="183"/>
+        <item x="175"/>
+        <item x="161"/>
+        <item x="165"/>
+        <item x="167"/>
+        <item x="169"/>
+        <item x="171"/>
+        <item x="163"/>
+        <item x="185"/>
+        <item x="189"/>
+        <item x="191"/>
+        <item x="193"/>
+        <item x="195"/>
+        <item x="187"/>
+        <item x="23"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="24"/>
+        <item x="17"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="18"/>
+        <item x="29"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="30"/>
+        <item x="35"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="36"/>
+        <item x="41"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="42"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="12"/>
+        <item x="47"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="48"/>
+        <item x="100"/>
+        <item x="104"/>
+        <item x="106"/>
+        <item x="108"/>
+        <item x="110"/>
+        <item x="102"/>
+        <item x="88"/>
+        <item x="92"/>
+        <item x="94"/>
+        <item x="96"/>
+        <item x="98"/>
+        <item x="90"/>
+        <item x="112"/>
+        <item x="116"/>
+        <item x="118"/>
+        <item x="120"/>
+        <item x="122"/>
+        <item x="114"/>
+        <item x="124"/>
+        <item x="128"/>
+        <item x="130"/>
+        <item x="132"/>
+        <item x="134"/>
+        <item x="126"/>
+        <item x="136"/>
+        <item x="140"/>
+        <item x="142"/>
+        <item x="144"/>
+        <item x="146"/>
+        <item x="138"/>
+        <item x="64"/>
+        <item x="68"/>
+        <item x="70"/>
+        <item x="72"/>
+        <item x="74"/>
+        <item x="66"/>
+        <item x="56"/>
+        <item x="58"/>
+        <item x="60"/>
+        <item x="62"/>
+        <item x="54"/>
+        <item x="76"/>
+        <item x="80"/>
+        <item x="82"/>
+        <item x="84"/>
+        <item x="86"/>
+        <item x="78"/>
+        <item x="148"/>
+        <item x="152"/>
+        <item x="154"/>
+        <item x="156"/>
+        <item x="158"/>
+        <item x="150"/>
+        <item x="101"/>
+        <item x="105"/>
+        <item x="107"/>
+        <item x="109"/>
+        <item x="111"/>
+        <item x="103"/>
+        <item x="89"/>
+        <item x="93"/>
+        <item x="95"/>
+        <item x="97"/>
+        <item x="99"/>
+        <item x="91"/>
+        <item x="113"/>
+        <item x="117"/>
+        <item x="119"/>
+        <item x="121"/>
+        <item x="123"/>
+        <item x="115"/>
+        <item x="125"/>
+        <item x="129"/>
+        <item x="131"/>
+        <item x="133"/>
+        <item x="135"/>
+        <item x="127"/>
+        <item x="137"/>
+        <item x="141"/>
+        <item x="143"/>
+        <item x="145"/>
+        <item x="147"/>
+        <item x="139"/>
+        <item x="65"/>
+        <item x="69"/>
+        <item x="71"/>
+        <item x="73"/>
+        <item x="75"/>
+        <item x="67"/>
+        <item x="53"/>
+        <item x="57"/>
+        <item x="59"/>
+        <item x="61"/>
+        <item x="63"/>
+        <item x="55"/>
+        <item x="77"/>
+        <item x="81"/>
+        <item x="83"/>
+        <item x="85"/>
+        <item x="87"/>
+        <item x="79"/>
+        <item x="149"/>
+        <item x="153"/>
+        <item x="155"/>
+        <item x="157"/>
+        <item x="159"/>
+        <item x="151"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="10">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Transcode Time (s)" fld="7" subtotal="average" baseField="2" baseItem="2" numFmtId="164"/>
+  </dataFields>
+  <formats count="10">
+    <format dxfId="24">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="23">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="22">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="21">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="20">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="19">
+      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="18">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="17">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="16">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="15">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="2">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A50195C7-F6C4-451B-9E01-A5D9F751ED02}" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="F48:G51" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Time Per GB" fld="8" subtotal="average" baseField="0" baseItem="1" numFmtId="164"/>
+  </dataFields>
+  <formats count="6">
+    <format dxfId="30">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="29">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="28">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="27">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="26">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="25">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{86F4D250-C3C7-481D-9A49-EB63AEA8CA1B}" name="PivotTable20" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="F17:I25" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="10">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item t="default" sd="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item sd="0" x="5"/>
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="252">
+        <item x="208"/>
+        <item x="211"/>
+        <item x="213"/>
+        <item x="215"/>
+        <item x="217"/>
+        <item x="209"/>
+        <item x="196"/>
+        <item x="200"/>
+        <item x="202"/>
+        <item x="204"/>
+        <item x="206"/>
+        <item x="198"/>
+        <item x="219"/>
+        <item x="223"/>
+        <item x="225"/>
+        <item x="227"/>
+        <item x="229"/>
+        <item x="221"/>
+        <item x="231"/>
+        <item x="236"/>
+        <item x="238"/>
+        <item x="240"/>
+        <item x="242"/>
+        <item x="233"/>
+        <item x="244"/>
+        <item x="248"/>
+        <item x="250"/>
+        <item x="246"/>
+        <item x="172"/>
+        <item x="176"/>
+        <item x="178"/>
+        <item x="180"/>
+        <item x="182"/>
+        <item x="174"/>
+        <item x="160"/>
+        <item x="164"/>
+        <item x="166"/>
+        <item x="168"/>
+        <item x="170"/>
+        <item x="162"/>
+        <item x="184"/>
+        <item x="188"/>
+        <item x="190"/>
+        <item x="192"/>
+        <item x="194"/>
+        <item x="186"/>
+        <item x="234"/>
+        <item x="212"/>
+        <item x="214"/>
+        <item x="216"/>
+        <item x="218"/>
+        <item x="210"/>
+        <item x="197"/>
+        <item x="201"/>
+        <item x="203"/>
+        <item x="205"/>
+        <item x="207"/>
+        <item x="199"/>
+        <item x="220"/>
+        <item x="224"/>
+        <item x="226"/>
+        <item x="228"/>
+        <item x="230"/>
+        <item x="222"/>
+        <item x="232"/>
+        <item x="237"/>
+        <item x="239"/>
+        <item x="241"/>
+        <item x="243"/>
+        <item x="235"/>
+        <item x="245"/>
+        <item x="249"/>
+        <item x="247"/>
+        <item x="173"/>
+        <item x="177"/>
+        <item x="179"/>
+        <item x="181"/>
+        <item x="183"/>
+        <item x="175"/>
+        <item x="161"/>
+        <item x="165"/>
+        <item x="167"/>
+        <item x="169"/>
+        <item x="171"/>
+        <item x="163"/>
+        <item x="185"/>
+        <item x="189"/>
+        <item x="191"/>
+        <item x="193"/>
+        <item x="195"/>
+        <item x="187"/>
+        <item x="23"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="24"/>
+        <item x="17"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="18"/>
+        <item x="29"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="30"/>
+        <item x="35"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="36"/>
+        <item x="41"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="42"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="12"/>
+        <item x="47"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="48"/>
+        <item x="100"/>
+        <item x="104"/>
+        <item x="106"/>
+        <item x="108"/>
+        <item x="110"/>
+        <item x="102"/>
+        <item x="88"/>
+        <item x="92"/>
+        <item x="94"/>
+        <item x="96"/>
+        <item x="98"/>
+        <item x="90"/>
+        <item x="112"/>
+        <item x="116"/>
+        <item x="118"/>
+        <item x="120"/>
+        <item x="122"/>
+        <item x="114"/>
+        <item x="124"/>
+        <item x="128"/>
+        <item x="130"/>
+        <item x="132"/>
+        <item x="134"/>
+        <item x="126"/>
+        <item x="136"/>
+        <item x="140"/>
+        <item x="142"/>
+        <item x="144"/>
+        <item x="146"/>
+        <item x="138"/>
+        <item x="64"/>
+        <item x="68"/>
+        <item x="70"/>
+        <item x="72"/>
+        <item x="74"/>
+        <item x="66"/>
+        <item x="56"/>
+        <item x="58"/>
+        <item x="60"/>
+        <item x="62"/>
+        <item x="54"/>
+        <item x="76"/>
+        <item x="80"/>
+        <item x="82"/>
+        <item x="84"/>
+        <item x="86"/>
+        <item x="78"/>
+        <item x="148"/>
+        <item x="152"/>
+        <item x="154"/>
+        <item x="156"/>
+        <item x="158"/>
+        <item x="150"/>
+        <item x="101"/>
+        <item x="105"/>
+        <item x="107"/>
+        <item x="109"/>
+        <item x="111"/>
+        <item x="103"/>
+        <item x="89"/>
+        <item x="93"/>
+        <item x="95"/>
+        <item x="97"/>
+        <item x="99"/>
+        <item x="91"/>
+        <item x="113"/>
+        <item x="117"/>
+        <item x="119"/>
+        <item x="121"/>
+        <item x="123"/>
+        <item x="115"/>
+        <item x="125"/>
+        <item x="129"/>
+        <item x="131"/>
+        <item x="133"/>
+        <item x="135"/>
+        <item x="127"/>
+        <item x="137"/>
+        <item x="141"/>
+        <item x="143"/>
+        <item x="145"/>
+        <item x="147"/>
+        <item x="139"/>
+        <item x="65"/>
+        <item x="69"/>
+        <item x="71"/>
+        <item x="73"/>
+        <item x="75"/>
+        <item x="67"/>
+        <item x="53"/>
+        <item x="57"/>
+        <item x="59"/>
+        <item x="61"/>
+        <item x="63"/>
+        <item x="55"/>
+        <item x="77"/>
+        <item x="81"/>
+        <item x="83"/>
+        <item x="85"/>
+        <item x="87"/>
+        <item x="79"/>
+        <item x="149"/>
+        <item x="153"/>
+        <item x="155"/>
+        <item x="157"/>
+        <item x="159"/>
+        <item x="151"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="3"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Output File Size" fld="6" subtotal="average" baseField="3" baseItem="0"/>
+  </dataFields>
+  <formats count="9">
+    <format dxfId="39">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="38">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="37">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="36">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="35">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="34">
+      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="33">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="32">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="31">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2B25D277-75F4-4EB1-A673-FD79F812B417}" name="PivotTable19" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A18:D29" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
@@ -20234,1385 +21612,6 @@
     <dataField name="Average of Output File Size" fld="6" subtotal="average" baseField="3" baseItem="0"/>
   </dataFields>
   <formats count="9">
-    <format dxfId="8">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="7">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="6">
-      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="5">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
-    </format>
-    <format dxfId="4">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="3">
-      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="2">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="1">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="0">
-      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FEB77646-3DBA-4492-8253-31CBB347E50E}" name="PivotTable14" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="F39:H46" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="9">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="5"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Input File Size" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Output File Size" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="6">
-    <format dxfId="14">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="13">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="12">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="11">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="10">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="9">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="2">
-            <x v="0"/>
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A0A28DC8-6D37-401F-9D67-74AD0D675A0F}" name="PivotTable10" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="F29:I37" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="9">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="10">
-        <item sd="0" x="4"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="5"/>
-        <item sd="0" x="6"/>
-        <item sd="0" x="7"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="0"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="8"/>
-        <item t="default" sd="0"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item sd="0" x="5"/>
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="252">
-        <item x="208"/>
-        <item x="211"/>
-        <item x="213"/>
-        <item x="215"/>
-        <item x="217"/>
-        <item x="209"/>
-        <item x="196"/>
-        <item x="200"/>
-        <item x="202"/>
-        <item x="204"/>
-        <item x="206"/>
-        <item x="198"/>
-        <item x="219"/>
-        <item x="223"/>
-        <item x="225"/>
-        <item x="227"/>
-        <item x="229"/>
-        <item x="221"/>
-        <item x="231"/>
-        <item x="236"/>
-        <item x="238"/>
-        <item x="240"/>
-        <item x="242"/>
-        <item x="233"/>
-        <item x="244"/>
-        <item x="248"/>
-        <item x="250"/>
-        <item x="246"/>
-        <item x="172"/>
-        <item x="176"/>
-        <item x="178"/>
-        <item x="180"/>
-        <item x="182"/>
-        <item x="174"/>
-        <item x="160"/>
-        <item x="164"/>
-        <item x="166"/>
-        <item x="168"/>
-        <item x="170"/>
-        <item x="162"/>
-        <item x="184"/>
-        <item x="188"/>
-        <item x="190"/>
-        <item x="192"/>
-        <item x="194"/>
-        <item x="186"/>
-        <item x="234"/>
-        <item x="212"/>
-        <item x="214"/>
-        <item x="216"/>
-        <item x="218"/>
-        <item x="210"/>
-        <item x="197"/>
-        <item x="201"/>
-        <item x="203"/>
-        <item x="205"/>
-        <item x="207"/>
-        <item x="199"/>
-        <item x="220"/>
-        <item x="224"/>
-        <item x="226"/>
-        <item x="228"/>
-        <item x="230"/>
-        <item x="222"/>
-        <item x="232"/>
-        <item x="237"/>
-        <item x="239"/>
-        <item x="241"/>
-        <item x="243"/>
-        <item x="235"/>
-        <item x="245"/>
-        <item x="249"/>
-        <item x="247"/>
-        <item x="173"/>
-        <item x="177"/>
-        <item x="179"/>
-        <item x="181"/>
-        <item x="183"/>
-        <item x="175"/>
-        <item x="161"/>
-        <item x="165"/>
-        <item x="167"/>
-        <item x="169"/>
-        <item x="171"/>
-        <item x="163"/>
-        <item x="185"/>
-        <item x="189"/>
-        <item x="191"/>
-        <item x="193"/>
-        <item x="195"/>
-        <item x="187"/>
-        <item x="23"/>
-        <item x="25"/>
-        <item x="26"/>
-        <item x="27"/>
-        <item x="28"/>
-        <item x="24"/>
-        <item x="17"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="18"/>
-        <item x="29"/>
-        <item x="31"/>
-        <item x="32"/>
-        <item x="33"/>
-        <item x="34"/>
-        <item x="30"/>
-        <item x="35"/>
-        <item x="37"/>
-        <item x="38"/>
-        <item x="39"/>
-        <item x="40"/>
-        <item x="36"/>
-        <item x="41"/>
-        <item x="43"/>
-        <item x="44"/>
-        <item x="45"/>
-        <item x="46"/>
-        <item x="42"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="11"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="12"/>
-        <item x="47"/>
-        <item x="49"/>
-        <item x="50"/>
-        <item x="51"/>
-        <item x="52"/>
-        <item x="48"/>
-        <item x="100"/>
-        <item x="104"/>
-        <item x="106"/>
-        <item x="108"/>
-        <item x="110"/>
-        <item x="102"/>
-        <item x="88"/>
-        <item x="92"/>
-        <item x="94"/>
-        <item x="96"/>
-        <item x="98"/>
-        <item x="90"/>
-        <item x="112"/>
-        <item x="116"/>
-        <item x="118"/>
-        <item x="120"/>
-        <item x="122"/>
-        <item x="114"/>
-        <item x="124"/>
-        <item x="128"/>
-        <item x="130"/>
-        <item x="132"/>
-        <item x="134"/>
-        <item x="126"/>
-        <item x="136"/>
-        <item x="140"/>
-        <item x="142"/>
-        <item x="144"/>
-        <item x="146"/>
-        <item x="138"/>
-        <item x="64"/>
-        <item x="68"/>
-        <item x="70"/>
-        <item x="72"/>
-        <item x="74"/>
-        <item x="66"/>
-        <item x="56"/>
-        <item x="58"/>
-        <item x="60"/>
-        <item x="62"/>
-        <item x="54"/>
-        <item x="76"/>
-        <item x="80"/>
-        <item x="82"/>
-        <item x="84"/>
-        <item x="86"/>
-        <item x="78"/>
-        <item x="148"/>
-        <item x="152"/>
-        <item x="154"/>
-        <item x="156"/>
-        <item x="158"/>
-        <item x="150"/>
-        <item x="101"/>
-        <item x="105"/>
-        <item x="107"/>
-        <item x="109"/>
-        <item x="111"/>
-        <item x="103"/>
-        <item x="89"/>
-        <item x="93"/>
-        <item x="95"/>
-        <item x="97"/>
-        <item x="99"/>
-        <item x="91"/>
-        <item x="113"/>
-        <item x="117"/>
-        <item x="119"/>
-        <item x="121"/>
-        <item x="123"/>
-        <item x="115"/>
-        <item x="125"/>
-        <item x="129"/>
-        <item x="131"/>
-        <item x="133"/>
-        <item x="135"/>
-        <item x="127"/>
-        <item x="137"/>
-        <item x="141"/>
-        <item x="143"/>
-        <item x="145"/>
-        <item x="147"/>
-        <item x="139"/>
-        <item x="65"/>
-        <item x="69"/>
-        <item x="71"/>
-        <item x="73"/>
-        <item x="75"/>
-        <item x="67"/>
-        <item x="53"/>
-        <item x="57"/>
-        <item x="59"/>
-        <item x="61"/>
-        <item x="63"/>
-        <item x="55"/>
-        <item x="77"/>
-        <item x="81"/>
-        <item x="83"/>
-        <item x="85"/>
-        <item x="87"/>
-        <item x="79"/>
-        <item x="149"/>
-        <item x="153"/>
-        <item x="155"/>
-        <item x="157"/>
-        <item x="159"/>
-        <item x="151"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="3"/>
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Time Per GB" fld="8" subtotal="average" baseField="3" baseItem="5" numFmtId="164"/>
-  </dataFields>
-  <formats count="9">
-    <format dxfId="23">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="22">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="21">
-      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="20">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
-    </format>
-    <format dxfId="19">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="18">
-      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0"/>
-    </format>
-    <format dxfId="17">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="16">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="15">
-      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E287444A-7E03-49CE-AE53-6E5021066FC9}" name="PivotTable6" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
-  <location ref="A2:D13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="10">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="10">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item sd="0" x="6"/>
-        <item sd="0" x="7"/>
-        <item sd="0" x="8"/>
-        <item t="default" sd="0"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="252">
-        <item x="208"/>
-        <item x="211"/>
-        <item x="213"/>
-        <item x="215"/>
-        <item x="217"/>
-        <item x="209"/>
-        <item x="196"/>
-        <item x="200"/>
-        <item x="202"/>
-        <item x="204"/>
-        <item x="206"/>
-        <item x="198"/>
-        <item x="219"/>
-        <item x="223"/>
-        <item x="225"/>
-        <item x="227"/>
-        <item x="229"/>
-        <item x="221"/>
-        <item x="231"/>
-        <item x="236"/>
-        <item x="238"/>
-        <item x="240"/>
-        <item x="242"/>
-        <item x="233"/>
-        <item x="244"/>
-        <item x="248"/>
-        <item x="250"/>
-        <item x="246"/>
-        <item x="172"/>
-        <item x="176"/>
-        <item x="178"/>
-        <item x="180"/>
-        <item x="182"/>
-        <item x="174"/>
-        <item x="160"/>
-        <item x="164"/>
-        <item x="166"/>
-        <item x="168"/>
-        <item x="170"/>
-        <item x="162"/>
-        <item x="184"/>
-        <item x="188"/>
-        <item x="190"/>
-        <item x="192"/>
-        <item x="194"/>
-        <item x="186"/>
-        <item x="234"/>
-        <item x="212"/>
-        <item x="214"/>
-        <item x="216"/>
-        <item x="218"/>
-        <item x="210"/>
-        <item x="197"/>
-        <item x="201"/>
-        <item x="203"/>
-        <item x="205"/>
-        <item x="207"/>
-        <item x="199"/>
-        <item x="220"/>
-        <item x="224"/>
-        <item x="226"/>
-        <item x="228"/>
-        <item x="230"/>
-        <item x="222"/>
-        <item x="232"/>
-        <item x="237"/>
-        <item x="239"/>
-        <item x="241"/>
-        <item x="243"/>
-        <item x="235"/>
-        <item x="245"/>
-        <item x="249"/>
-        <item x="247"/>
-        <item x="173"/>
-        <item x="177"/>
-        <item x="179"/>
-        <item x="181"/>
-        <item x="183"/>
-        <item x="175"/>
-        <item x="161"/>
-        <item x="165"/>
-        <item x="167"/>
-        <item x="169"/>
-        <item x="171"/>
-        <item x="163"/>
-        <item x="185"/>
-        <item x="189"/>
-        <item x="191"/>
-        <item x="193"/>
-        <item x="195"/>
-        <item x="187"/>
-        <item x="23"/>
-        <item x="25"/>
-        <item x="26"/>
-        <item x="27"/>
-        <item x="28"/>
-        <item x="24"/>
-        <item x="17"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="18"/>
-        <item x="29"/>
-        <item x="31"/>
-        <item x="32"/>
-        <item x="33"/>
-        <item x="34"/>
-        <item x="30"/>
-        <item x="35"/>
-        <item x="37"/>
-        <item x="38"/>
-        <item x="39"/>
-        <item x="40"/>
-        <item x="36"/>
-        <item x="41"/>
-        <item x="43"/>
-        <item x="44"/>
-        <item x="45"/>
-        <item x="46"/>
-        <item x="42"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="11"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="12"/>
-        <item x="47"/>
-        <item x="49"/>
-        <item x="50"/>
-        <item x="51"/>
-        <item x="52"/>
-        <item x="48"/>
-        <item x="100"/>
-        <item x="104"/>
-        <item x="106"/>
-        <item x="108"/>
-        <item x="110"/>
-        <item x="102"/>
-        <item x="88"/>
-        <item x="92"/>
-        <item x="94"/>
-        <item x="96"/>
-        <item x="98"/>
-        <item x="90"/>
-        <item x="112"/>
-        <item x="116"/>
-        <item x="118"/>
-        <item x="120"/>
-        <item x="122"/>
-        <item x="114"/>
-        <item x="124"/>
-        <item x="128"/>
-        <item x="130"/>
-        <item x="132"/>
-        <item x="134"/>
-        <item x="126"/>
-        <item x="136"/>
-        <item x="140"/>
-        <item x="142"/>
-        <item x="144"/>
-        <item x="146"/>
-        <item x="138"/>
-        <item x="64"/>
-        <item x="68"/>
-        <item x="70"/>
-        <item x="72"/>
-        <item x="74"/>
-        <item x="66"/>
-        <item x="56"/>
-        <item x="58"/>
-        <item x="60"/>
-        <item x="62"/>
-        <item x="54"/>
-        <item x="76"/>
-        <item x="80"/>
-        <item x="82"/>
-        <item x="84"/>
-        <item x="86"/>
-        <item x="78"/>
-        <item x="148"/>
-        <item x="152"/>
-        <item x="154"/>
-        <item x="156"/>
-        <item x="158"/>
-        <item x="150"/>
-        <item x="101"/>
-        <item x="105"/>
-        <item x="107"/>
-        <item x="109"/>
-        <item x="111"/>
-        <item x="103"/>
-        <item x="89"/>
-        <item x="93"/>
-        <item x="95"/>
-        <item x="97"/>
-        <item x="99"/>
-        <item x="91"/>
-        <item x="113"/>
-        <item x="117"/>
-        <item x="119"/>
-        <item x="121"/>
-        <item x="123"/>
-        <item x="115"/>
-        <item x="125"/>
-        <item x="129"/>
-        <item x="131"/>
-        <item x="133"/>
-        <item x="135"/>
-        <item x="127"/>
-        <item x="137"/>
-        <item x="141"/>
-        <item x="143"/>
-        <item x="145"/>
-        <item x="147"/>
-        <item x="139"/>
-        <item x="65"/>
-        <item x="69"/>
-        <item x="71"/>
-        <item x="73"/>
-        <item x="75"/>
-        <item x="67"/>
-        <item x="53"/>
-        <item x="57"/>
-        <item x="59"/>
-        <item x="61"/>
-        <item x="63"/>
-        <item x="55"/>
-        <item x="77"/>
-        <item x="81"/>
-        <item x="83"/>
-        <item x="85"/>
-        <item x="87"/>
-        <item x="79"/>
-        <item x="149"/>
-        <item x="153"/>
-        <item x="155"/>
-        <item x="157"/>
-        <item x="159"/>
-        <item x="151"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="2"/>
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="10">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Transcode Time (s)" fld="7" subtotal="average" baseField="2" baseItem="2" numFmtId="164"/>
-  </dataFields>
-  <formats count="10">
-    <format dxfId="33">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="32">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="31">
-      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="30">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
-    </format>
-    <format dxfId="29">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="28">
-      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="27">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="2" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="26">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="25">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="24">
-      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="2">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A50195C7-F6C4-451B-9E01-A5D9F751ED02}" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="F48:G51" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="10">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Time Per GB" fld="8" subtotal="average" baseField="0" baseItem="1" numFmtId="164"/>
-  </dataFields>
-  <formats count="6">
-    <format dxfId="39">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="38">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="37">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="36">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="35">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="34">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{86F4D250-C3C7-481D-9A49-EB63AEA8CA1B}" name="PivotTable20" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="F17:I25" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="9">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="10">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item sd="0" x="6"/>
-        <item sd="0" x="7"/>
-        <item sd="0" x="8"/>
-        <item t="default" sd="0"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item sd="0" x="5"/>
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="252">
-        <item x="208"/>
-        <item x="211"/>
-        <item x="213"/>
-        <item x="215"/>
-        <item x="217"/>
-        <item x="209"/>
-        <item x="196"/>
-        <item x="200"/>
-        <item x="202"/>
-        <item x="204"/>
-        <item x="206"/>
-        <item x="198"/>
-        <item x="219"/>
-        <item x="223"/>
-        <item x="225"/>
-        <item x="227"/>
-        <item x="229"/>
-        <item x="221"/>
-        <item x="231"/>
-        <item x="236"/>
-        <item x="238"/>
-        <item x="240"/>
-        <item x="242"/>
-        <item x="233"/>
-        <item x="244"/>
-        <item x="248"/>
-        <item x="250"/>
-        <item x="246"/>
-        <item x="172"/>
-        <item x="176"/>
-        <item x="178"/>
-        <item x="180"/>
-        <item x="182"/>
-        <item x="174"/>
-        <item x="160"/>
-        <item x="164"/>
-        <item x="166"/>
-        <item x="168"/>
-        <item x="170"/>
-        <item x="162"/>
-        <item x="184"/>
-        <item x="188"/>
-        <item x="190"/>
-        <item x="192"/>
-        <item x="194"/>
-        <item x="186"/>
-        <item x="234"/>
-        <item x="212"/>
-        <item x="214"/>
-        <item x="216"/>
-        <item x="218"/>
-        <item x="210"/>
-        <item x="197"/>
-        <item x="201"/>
-        <item x="203"/>
-        <item x="205"/>
-        <item x="207"/>
-        <item x="199"/>
-        <item x="220"/>
-        <item x="224"/>
-        <item x="226"/>
-        <item x="228"/>
-        <item x="230"/>
-        <item x="222"/>
-        <item x="232"/>
-        <item x="237"/>
-        <item x="239"/>
-        <item x="241"/>
-        <item x="243"/>
-        <item x="235"/>
-        <item x="245"/>
-        <item x="249"/>
-        <item x="247"/>
-        <item x="173"/>
-        <item x="177"/>
-        <item x="179"/>
-        <item x="181"/>
-        <item x="183"/>
-        <item x="175"/>
-        <item x="161"/>
-        <item x="165"/>
-        <item x="167"/>
-        <item x="169"/>
-        <item x="171"/>
-        <item x="163"/>
-        <item x="185"/>
-        <item x="189"/>
-        <item x="191"/>
-        <item x="193"/>
-        <item x="195"/>
-        <item x="187"/>
-        <item x="23"/>
-        <item x="25"/>
-        <item x="26"/>
-        <item x="27"/>
-        <item x="28"/>
-        <item x="24"/>
-        <item x="17"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="18"/>
-        <item x="29"/>
-        <item x="31"/>
-        <item x="32"/>
-        <item x="33"/>
-        <item x="34"/>
-        <item x="30"/>
-        <item x="35"/>
-        <item x="37"/>
-        <item x="38"/>
-        <item x="39"/>
-        <item x="40"/>
-        <item x="36"/>
-        <item x="41"/>
-        <item x="43"/>
-        <item x="44"/>
-        <item x="45"/>
-        <item x="46"/>
-        <item x="42"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="11"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="12"/>
-        <item x="47"/>
-        <item x="49"/>
-        <item x="50"/>
-        <item x="51"/>
-        <item x="52"/>
-        <item x="48"/>
-        <item x="100"/>
-        <item x="104"/>
-        <item x="106"/>
-        <item x="108"/>
-        <item x="110"/>
-        <item x="102"/>
-        <item x="88"/>
-        <item x="92"/>
-        <item x="94"/>
-        <item x="96"/>
-        <item x="98"/>
-        <item x="90"/>
-        <item x="112"/>
-        <item x="116"/>
-        <item x="118"/>
-        <item x="120"/>
-        <item x="122"/>
-        <item x="114"/>
-        <item x="124"/>
-        <item x="128"/>
-        <item x="130"/>
-        <item x="132"/>
-        <item x="134"/>
-        <item x="126"/>
-        <item x="136"/>
-        <item x="140"/>
-        <item x="142"/>
-        <item x="144"/>
-        <item x="146"/>
-        <item x="138"/>
-        <item x="64"/>
-        <item x="68"/>
-        <item x="70"/>
-        <item x="72"/>
-        <item x="74"/>
-        <item x="66"/>
-        <item x="56"/>
-        <item x="58"/>
-        <item x="60"/>
-        <item x="62"/>
-        <item x="54"/>
-        <item x="76"/>
-        <item x="80"/>
-        <item x="82"/>
-        <item x="84"/>
-        <item x="86"/>
-        <item x="78"/>
-        <item x="148"/>
-        <item x="152"/>
-        <item x="154"/>
-        <item x="156"/>
-        <item x="158"/>
-        <item x="150"/>
-        <item x="101"/>
-        <item x="105"/>
-        <item x="107"/>
-        <item x="109"/>
-        <item x="111"/>
-        <item x="103"/>
-        <item x="89"/>
-        <item x="93"/>
-        <item x="95"/>
-        <item x="97"/>
-        <item x="99"/>
-        <item x="91"/>
-        <item x="113"/>
-        <item x="117"/>
-        <item x="119"/>
-        <item x="121"/>
-        <item x="123"/>
-        <item x="115"/>
-        <item x="125"/>
-        <item x="129"/>
-        <item x="131"/>
-        <item x="133"/>
-        <item x="135"/>
-        <item x="127"/>
-        <item x="137"/>
-        <item x="141"/>
-        <item x="143"/>
-        <item x="145"/>
-        <item x="147"/>
-        <item x="139"/>
-        <item x="65"/>
-        <item x="69"/>
-        <item x="71"/>
-        <item x="73"/>
-        <item x="75"/>
-        <item x="67"/>
-        <item x="53"/>
-        <item x="57"/>
-        <item x="59"/>
-        <item x="61"/>
-        <item x="63"/>
-        <item x="55"/>
-        <item x="77"/>
-        <item x="81"/>
-        <item x="83"/>
-        <item x="85"/>
-        <item x="87"/>
-        <item x="79"/>
-        <item x="149"/>
-        <item x="153"/>
-        <item x="155"/>
-        <item x="157"/>
-        <item x="159"/>
-        <item x="151"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="3"/>
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Output File Size" fld="6" subtotal="average" baseField="3" baseItem="0"/>
-  </dataFields>
-  <formats count="9">
     <format dxfId="48">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
@@ -21629,7 +21628,7 @@
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
     <format dxfId="43">
-      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
     <format dxfId="42">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
@@ -21996,7 +21995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D5C156-544C-4B79-8085-8E51A005FEBE}">
   <dimension ref="B3:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -34712,8 +34711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CDEEDA3-D005-4D7D-B23B-831CED25EFEB}">
   <dimension ref="B2:P30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34727,65 +34726,65 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>0</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>5</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>10</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="8">
         <v>15</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <v>20</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="8">
         <v>25</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -34845,7 +34844,7 @@
   "")</f>
         <v>154514293</v>
       </c>
-      <c r="I5" s="11" cm="1">
+      <c r="I5" s="10" cm="1">
         <f t="array" ref="I5">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
@@ -34909,7 +34908,7 @@
   "")</f>
         <v>167176724</v>
       </c>
-      <c r="I6" s="11" cm="1">
+      <c r="I6" s="10" cm="1">
         <f t="array" ref="I6">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
@@ -34973,7 +34972,7 @@
   "")</f>
         <v>163493670</v>
       </c>
-      <c r="I7" s="11" cm="1">
+      <c r="I7" s="10" cm="1">
         <f t="array" ref="I7">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
@@ -35037,7 +35036,7 @@
   "")</f>
         <v>163462297</v>
       </c>
-      <c r="I8" s="11" cm="1">
+      <c r="I8" s="10" cm="1">
         <f t="array" ref="I8">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
@@ -35101,7 +35100,7 @@
   "")</f>
         <v>165475610</v>
       </c>
-      <c r="I9" s="11" cm="1">
+      <c r="I9" s="10" cm="1">
         <f t="array" ref="I9">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
@@ -35165,7 +35164,7 @@
   "")</f>
         <v>169180586</v>
       </c>
-      <c r="I10" s="11" cm="1">
+      <c r="I10" s="10" cm="1">
         <f t="array" ref="I10">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
@@ -35229,7 +35228,7 @@
   "")</f>
         <v>180394129</v>
       </c>
-      <c r="I11" s="11" cm="1">
+      <c r="I11" s="10" cm="1">
         <f t="array" ref="I11">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
@@ -35293,7 +35292,7 @@
   "")</f>
         <v>180670604</v>
       </c>
-      <c r="I12" s="11" cm="1">
+      <c r="I12" s="10" cm="1">
         <f t="array" ref="I12">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
@@ -35357,97 +35356,97 @@
   "")</f>
         <v>179916087</v>
       </c>
-      <c r="I13" s="11" cm="1">
+      <c r="I13" s="10" cm="1">
         <f t="array" ref="I13">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C14" s="11" cm="1">
+      <c r="C14" s="10" cm="1">
         <f t="array" ref="C14">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
-      <c r="D14" s="11" cm="1">
+      <c r="D14" s="10" cm="1">
         <f t="array" ref="D14">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
-      <c r="E14" s="11" cm="1">
+      <c r="E14" s="10" cm="1">
         <f t="array" ref="E14">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
-      <c r="F14" s="11" cm="1">
+      <c r="F14" s="10" cm="1">
         <f t="array" ref="F14">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
-      <c r="G14" s="11" cm="1">
+      <c r="G14" s="10" cm="1">
         <f t="array" ref="G14">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
-      <c r="H14" s="11" cm="1">
+      <c r="H14" s="10" cm="1">
         <f t="array" ref="H14">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
-      <c r="I14" s="11" cm="1">
+      <c r="I14" s="10" cm="1">
         <f t="array" ref="I14">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="11" t="s">
         <v>294</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="8">
         <v>0</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="8">
         <v>5</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="8">
         <v>10</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="8">
         <v>15</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="8">
         <v>20</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="8">
         <v>25</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" s="9" t="s">
         <v>109</v>
       </c>
     </row>
@@ -35509,7 +35508,7 @@
   "")</f>
         <v>22143.130336968035</v>
       </c>
-      <c r="I21" s="11" cm="1">
+      <c r="I21" s="10" cm="1">
         <f t="array" ref="I21">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
@@ -35572,7 +35571,7 @@
   "")</f>
         <v>24059.842442663768</v>
       </c>
-      <c r="I22" s="11" cm="1">
+      <c r="I22" s="10" cm="1">
         <f t="array" ref="I22">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
@@ -35635,7 +35634,7 @@
   "")</f>
         <v>26667.163302180739</v>
       </c>
-      <c r="I23" s="11" cm="1">
+      <c r="I23" s="10" cm="1">
         <f t="array" ref="I23">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
@@ -35698,7 +35697,7 @@
   "")</f>
         <v>29028.172235955597</v>
       </c>
-      <c r="I24" s="11" cm="1">
+      <c r="I24" s="10" cm="1">
         <f t="array" ref="I24">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
@@ -35761,7 +35760,7 @@
   "")</f>
         <v>31234.846482081917</v>
       </c>
-      <c r="I25" s="11" cm="1">
+      <c r="I25" s="10" cm="1">
         <f t="array" ref="I25">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
@@ -35824,7 +35823,7 @@
   "")</f>
         <v>34830.532917045079</v>
       </c>
-      <c r="I26" s="11" cm="1">
+      <c r="I26" s="10" cm="1">
         <f t="array" ref="I26">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
@@ -35887,7 +35886,7 @@
   "")</f>
         <v>43489.644255871397</v>
       </c>
-      <c r="I27" s="11" cm="1">
+      <c r="I27" s="10" cm="1">
         <f t="array" ref="I27">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
@@ -35950,7 +35949,7 @@
   "")</f>
         <v>104235.93320795988</v>
       </c>
-      <c r="I28" s="11" cm="1">
+      <c r="I28" s="10" cm="1">
         <f t="array" ref="I28">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
@@ -36013,40 +36012,40 @@
   "")</f>
         <v>208989.433247226</v>
       </c>
-      <c r="I29" s="11" cm="1">
+      <c r="I29" s="10" cm="1">
         <f t="array" ref="I29">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C30" s="11" cm="1">
+      <c r="C30" s="10" cm="1">
         <f t="array" ref="C30">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
-      <c r="D30" s="11" cm="1">
+      <c r="D30" s="10" cm="1">
         <f t="array" ref="D30">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
-      <c r="E30" s="11" cm="1">
+      <c r="E30" s="10" cm="1">
         <f t="array" ref="E30">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
-      <c r="F30" s="11" cm="1">
+      <c r="F30" s="10" cm="1">
         <f t="array" ref="F30">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
-      <c r="G30" s="11" cm="1">
+      <c r="G30" s="10" cm="1">
         <f t="array" ref="G30">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
-      <c r="H30" s="11" cm="1">
+      <c r="H30" s="10" cm="1">
         <f t="array" ref="H30">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
-      <c r="I30" s="11" cm="1">
+      <c r="I30" s="10" cm="1">
         <f t="array" ref="I30">_xlfn._xlws.FILTER(INTERNAL!$F$3:$F$5,'Graphs 1'!$C$3=INTERNAL!$E$3:$E$5,"")</f>
         <v>1282926107</v>
       </c>
@@ -36081,7 +36080,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4B75D22-A47C-4D4A-9070-CE9067E49D8D}">
-  <dimension ref="B2:H10"/>
+  <dimension ref="B2:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:F2"/>
@@ -36095,94 +36094,56 @@
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>289</v>
       </c>
       <c r="C2" t="s">
         <v>290</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="10">
         <v>1282926107</v>
       </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <v>7779270190</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <v>2170027841</v>
       </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>